<commit_message>
NFL Team Season with opponent statistics and CSV/Excel
</commit_message>
<xml_diff>
--- a/Data/NFLSeasonStatDescriptions.xlsx
+++ b/Data/NFLSeasonStatDescriptions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9285" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TeamNames" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
   <si>
     <t>NFLDB Stat</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>"17"</t>
+  </si>
+  <si>
+    <t>Rushing Touchdowns:6 points</t>
   </si>
 </sst>
 </file>
@@ -894,7 +897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1017,7 +1020,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>85</v>
       </c>
@@ -1092,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1200,9 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1229,7 +1234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
         <v>27</v>
@@ -1238,7 +1243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>29</v>
@@ -1247,7 +1252,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
         <v>12</v>
@@ -1256,7 +1261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
         <v>31</v>

</xml_diff>